<commit_message>
MT:  Finished DNRC 2015 State Water Plan
</commit_message>
<xml_diff>
--- a/Vocabularies/OR/or-sos-d.xlsx
+++ b/Vocabularies/OR/or-sos-d.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph/Desktop/WSWC/IoW/Vocabularies/OR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustus/Desktop/WSWC/IoW/Vocabularies/OR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B7AACC-E87A-1C47-BC0C-87BC150FB114}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D252AE0F-BB5A-5B4F-81ED-1C2867D1F7F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
+    <workbookView xWindow="960" yWindow="3840" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t>Term</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>A short section of definitions included in an annual report to the Oregon Secretary of State from the Oregon Water Resources Department</t>
+  </si>
+  <si>
+    <t>https://secure.sos.state.or.us/oard/displayDivisionRules.action?selectedDivision=3174</t>
   </si>
 </sst>
 </file>
@@ -853,7 +856,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -909,6 +912,9 @@
       <c r="E2" t="s">
         <v>69</v>
       </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
       <c r="G2" t="s">
         <v>26</v>
       </c>

</xml_diff>